<commit_message>
Updated footprints to 0805 packages
</commit_message>
<xml_diff>
--- a/Components/Qwiic_Adaptive_Switch_Input_BOM.xlsx
+++ b/Components/Qwiic_Adaptive_Switch_Input_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\Personal\Qwiic-Adaptive-Switch\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A7E4FC-CB10-4506-99A4-55F315B8FA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758B54A9-4B34-42A2-842B-0AEC5E130CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="1470" windowWidth="22980" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="1500" windowWidth="25455" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Qwiic_Adaptive_Switch_Input_BOM" sheetId="1" r:id="rId1"/>
@@ -78,27 +78,6 @@
     <t>QWIIC JST CONNECTOR - SMD 4-PIN</t>
   </si>
   <si>
-    <t>311-2.20KHRTR-ND</t>
-  </si>
-  <si>
-    <t>RC0603FR-072K2L</t>
-  </si>
-  <si>
-    <t>RES SMD 2.2K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>587-1245-2-ND</t>
-  </si>
-  <si>
-    <t>TMK107BJ104KA-T</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 25V X5R 0603</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/taiyo-yuden/TMK107BJ104KA-T/930597</t>
-  </si>
-  <si>
     <t>160-1436-2-ND</t>
   </si>
   <si>
@@ -162,42 +141,6 @@
     <t>4.7K</t>
   </si>
   <si>
-    <t>311-4.7KGRTR-ND</t>
-  </si>
-  <si>
-    <t>RC0603JR-074K7L</t>
-  </si>
-  <si>
-    <t>RES SMD 4.7K OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603JR-074K7L/726785</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603JR-0710KL/726700</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-10KGRTR-ND </t>
-  </si>
-  <si>
-    <t>RC0603JR-0710KL</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-071KL/726843</t>
-  </si>
-  <si>
-    <t>311-1.00KHRTR-ND</t>
-  </si>
-  <si>
-    <t>RC0603FR-071KL</t>
-  </si>
-  <si>
-    <t>RES SMD 1K OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
     <t>QWIIC JST</t>
   </si>
   <si>
@@ -210,9 +153,6 @@
     <t>Total Price (CAD)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/yageo/RC0603FR-072K2L/727016 </t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.digikey.ca/en/products/detail/sparkfun-electronics/PRT-14417/7652746 </t>
   </si>
   <si>
@@ -220,6 +160,66 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.ca/en/products/detail/cui-devices/SJ1-3513/738683 </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0805FR-072K2L/727676</t>
+  </si>
+  <si>
+    <t>RES 2.2K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RC0805FR-072K2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-2.20KCRCT-ND </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0805FR-0710KL/727535</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RC0805FR-0710KL</t>
+  </si>
+  <si>
+    <t>311-10.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0805JR-074K7L/728327</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 5% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RC0805JR-074K7L</t>
+  </si>
+  <si>
+    <t>311-4.7KARCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0805FR-071KL/727444</t>
+  </si>
+  <si>
+    <t>RES 1K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RC0805FR-071KL</t>
+  </si>
+  <si>
+    <t>311-1.00KCRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/avx-corporation/08053C104KAT2A/1116281</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V X7R 0805</t>
+  </si>
+  <si>
+    <t>08053C104KAT2A</t>
+  </si>
+  <si>
+    <t>478-3755-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1100,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,7 +1113,7 @@
     <col min="7" max="7" width="32.85546875" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="50.140625" customWidth="1"/>
+    <col min="10" max="10" width="77.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1127,7 +1127,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1139,10 +1139,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>6</v>
@@ -1177,7 +1177,7 @@
         <v>1.97</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1191,16 +1191,16 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1">
         <v>1.82</v>
@@ -1209,7 +1209,7 @@
         <v>1.82</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1220,10 +1220,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
@@ -1241,7 +1241,7 @@
         <v>0.69</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1252,19 +1252,19 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="H5" s="1">
         <v>0.15</v>
@@ -1273,7 +1273,7 @@
         <v>0.15</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1284,16 +1284,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>48</v>
@@ -1316,19 +1316,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H7" s="1">
         <v>0.15</v>
@@ -1337,7 +1337,7 @@
         <v>0.15</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1348,19 +1348,19 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H8" s="1">
         <v>0.15</v>
@@ -1369,7 +1369,7 @@
         <v>0.15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1380,19 +1380,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="H9" s="1">
         <v>0.14000000000000001</v>
@@ -1401,7 +1401,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1412,19 +1412,19 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H10" s="1">
         <v>0.33</v>
@@ -1433,12 +1433,12 @@
         <v>0.33</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H13" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I13" s="1">
         <f>H2*B2+H3*B3+H4*B4+H5*B5+H6*B6+H7*B7+H8*B8+H9*B9+H10*B10</f>

</xml_diff>

<commit_message>
Updated version 2.1 BOM
</commit_message>
<xml_diff>
--- a/Components/Qwiic_Adaptive_Switch_Input_BOM.xlsx
+++ b/Components/Qwiic_Adaptive_Switch_Input_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\Personal\Qwiic-Adaptive-Switch\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758B54A9-4B34-42A2-842B-0AEC5E130CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C290B40-3705-419A-97BE-0FF8D605B7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1500" windowWidth="25455" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4788" yWindow="552" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Qwiic_Adaptive_Switch_Input_BOM" sheetId="1" r:id="rId1"/>
@@ -126,18 +126,9 @@
     <t>2.2K</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
-    <t>R1,R2,R7,R8,R9</t>
-  </si>
-  <si>
-    <t>R5,R6</t>
-  </si>
-  <si>
     <t>4.7K</t>
   </si>
   <si>
@@ -220,6 +211,15 @@
   </si>
   <si>
     <t>478-3755-1-ND</t>
+  </si>
+  <si>
+    <t>R1,R2,R4,R5,R6</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R7,R8</t>
   </si>
 </sst>
 </file>
@@ -1099,24 +1099,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" customWidth="1"/>
+    <col min="7" max="7" width="32.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="77.85546875" customWidth="1"/>
+    <col min="10" max="10" width="77.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1139,16 +1139,16 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1177,10 +1177,10 @@
         <v>1.97</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1209,10 +1209,10 @@
         <v>1.82</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1220,10 +1220,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
@@ -1241,10 +1241,10 @@
         <v>0.69</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1252,19 +1252,19 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H5" s="1">
         <v>0.15</v>
@@ -1273,10 +1273,10 @@
         <v>0.15</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1284,19 +1284,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H6" s="1">
         <v>0.15</v>
@@ -1305,30 +1305,30 @@
         <v>0.15</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H7" s="1">
         <v>0.15</v>
@@ -1337,30 +1337,30 @@
         <v>0.15</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H8" s="1">
         <v>0.15</v>
@@ -1369,10 +1369,10 @@
         <v>0.15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1386,13 +1386,13 @@
         <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H9" s="1">
         <v>0.14000000000000001</v>
@@ -1401,10 +1401,10 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1436,20 +1436,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I13" s="1">
-        <f>H2*B2+H3*B3+H4*B4+H5*B5+H6*B6+H7*B7+H8*B8+H9*B9+H10*B10</f>
+        <f>H2*B2+H3*B3+H4*B4+H5*B5+H8*B8+H6*B6+H7*B7+H9*B9+H10*B10</f>
         <v>8.9600000000000009</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J8" r:id="rId1" xr:uid="{57F48D8A-3087-47C8-A385-FEC943BA2F89}"/>
-    <hyperlink ref="J7" r:id="rId2" xr:uid="{303FD325-93A2-4122-A17E-C111FE863494}"/>
-    <hyperlink ref="J6" r:id="rId3" xr:uid="{45ABB9EA-EB9F-4A28-9ABF-7C64A3A6F5DB}"/>
+    <hyperlink ref="J7" r:id="rId1" xr:uid="{57F48D8A-3087-47C8-A385-FEC943BA2F89}"/>
+    <hyperlink ref="J6" r:id="rId2" xr:uid="{303FD325-93A2-4122-A17E-C111FE863494}"/>
+    <hyperlink ref="J8" r:id="rId3" xr:uid="{45ABB9EA-EB9F-4A28-9ABF-7C64A3A6F5DB}"/>
     <hyperlink ref="J9" r:id="rId4" xr:uid="{9B4361CF-880F-4767-81AA-95457881CD70}"/>
     <hyperlink ref="J10" r:id="rId5" xr:uid="{3E4978E0-C4E0-49A4-8EB1-E99414799B0D}"/>
     <hyperlink ref="J5" r:id="rId6" xr:uid="{26D89B83-EC94-41FB-89FF-57777394B326}"/>

</xml_diff>